<commit_message>
fix sample edge json
</commit_message>
<xml_diff>
--- a/samples/transform/hough_image_grayscale_accumulator.xlsx
+++ b/samples/transform/hough_image_grayscale_accumulator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kushn\projects\cv-workbench\samples\transform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9773033-A2F8-4D96-971F-C41CD8CC113E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDD3D37-EC72-4CC8-8077-71EDB4AEC914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{EAD2CA60-0884-4BE1-9039-2EF307E7835B}"/>
   </bookViews>
@@ -542,10 +542,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -969,7 +968,7 @@
       <selection activeCell="BQ11" sqref="BQ11"/>
       <selection pane="topRight" activeCell="EK9" sqref="EK9"/>
       <selection pane="bottomLeft" activeCell="A40" sqref="A40"/>
-      <selection pane="bottomRight" activeCell="DN104" sqref="DN104"/>
+      <selection pane="bottomRight" activeCell="EK39" sqref="EK39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20612,7 +20611,7 @@
       <c r="EJ39">
         <v>459858</v>
       </c>
-      <c r="EK39" s="2">
+      <c r="EK39" s="1">
         <v>2267697</v>
       </c>
       <c r="EL39">

</xml_diff>